<commit_message>
Hoàn thành chức năng điểm danh vào, ra.
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/Mẫu import sinh viên.xlsx
+++ b/Sources/DD_RFID/public/download/Mẫu import sinh viên.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>mssv</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>- Tốc độ import sẽ chậm dần theo thứ tự định dạng như sau: csv (nhanh nhất) &gt; xls &gt; xlsx</t>
   </si>
 </sst>
 </file>
@@ -481,13 +484,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -544,13 +547,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -607,13 +610,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -670,13 +673,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -732,13 +735,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Q44"/>
+  <dimension ref="B3:Q45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,28 +1209,28 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1245,10 +1248,10 @@
       <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
-      <c r="C12" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1264,10 +1267,10 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
       <c r="C13" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1284,9 +1287,11 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1662,11 +1667,9 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="9"/>
     </row>
-    <row r="35" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
-      <c r="C35" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1685,7 +1688,7 @@
     <row r="36" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1702,9 +1705,11 @@
       <c r="P36" s="8"/>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
+      <c r="C37" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1829,22 +1834,40 @@
       <c r="Q43" s="9"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="16"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="9"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>